<commit_message>
update of princing values and updates on the standard table
</commit_message>
<xml_diff>
--- a/static/padrao-tabela.xlsx
+++ b/static/padrao-tabela.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">FRETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">← Não mexer nessa linha</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -121,6 +124,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -140,13 +147,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.43"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -159,10 +169,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>

</xml_diff>